<commit_message>
[imp]add unit test for sys setting
</commit_message>
<xml_diff>
--- a/src/test/resources/script/db/init-data/choerodon-sys-setting.xlsx
+++ b/src/test/resources/script/db/init-data/choerodon-sys-setting.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projcect\hzero-iam\src\main\resources\script\db\init-data\hzero_platform\hzero_platform\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projcect\iam\hzero-iam\src\test\resources\script\db\init-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39BA0309-417C-45F8-9B00-91E7D8335BEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0E97B3-4C17-4F7F-8966-17834C57442F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="597" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="71">
   <si>
     <r>
       <rPr>
@@ -2049,23 +2049,40 @@
     <phoneticPr fontId="23" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>t</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>rue</t>
-    </r>
+    <t>*</t>
     <phoneticPr fontId="23" type="noConversion"/>
   </si>
   <si>
-    <t>forceModifyPassword</t>
+    <t>autoCleanEmailRecord</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>autoCleanEmailRecordInterval</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>autoCleanWebhookRecord</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>autoCleanWebhookRecordInterval</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>autoCleanSagaInstance</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>autoCleanSagaInstanceInterval</t>
+  </si>
+  <si>
+    <t>retainFailedSagaInstance</t>
+  </si>
+  <si>
+    <t>TRUE</t>
     <phoneticPr fontId="23" type="noConversion"/>
   </si>
 </sst>
@@ -2073,7 +2090,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -2227,6 +2244,12 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF6A8759"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -2366,7 +2389,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2436,6 +2459,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2821,11 +2853,11 @@
   <sheetData>
     <row r="1" spans="1:8" ht="64.5" customHeight="1">
       <c r="A1" s="8"/>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
       <c r="F1" s="22"/>
       <c r="G1" s="22"/>
       <c r="H1" s="22"/>
@@ -2834,21 +2866,21 @@
       <c r="E2" s="19"/>
     </row>
     <row r="3" spans="1:8" ht="49.5" customHeight="1">
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="37"/>
-      <c r="E3" s="39" t="s">
+      <c r="D3" s="40"/>
+      <c r="E3" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
     </row>
     <row r="4" spans="1:8" ht="18">
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="40"/>
+      <c r="D4" s="43"/>
       <c r="E4" s="23" t="s">
         <v>4</v>
       </c>
@@ -2959,11 +2991,11 @@
       </c>
     </row>
     <row r="19" spans="3:5">
-      <c r="C19" s="41" t="s">
+      <c r="C19" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
     </row>
     <row r="20" spans="3:5" ht="18">
       <c r="C20" s="18" t="s">
@@ -3001,19 +3033,19 @@
       <c r="C25" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="37" t="s">
+      <c r="D25" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="37"/>
+      <c r="E25" s="40"/>
     </row>
     <row r="26" spans="3:5" ht="14.25" customHeight="1">
       <c r="C26" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="37" t="s">
+      <c r="D26" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="37"/>
+      <c r="E26" s="40"/>
     </row>
     <row r="27" spans="3:5" ht="51.75">
       <c r="C27" s="21" t="s">
@@ -3038,10 +3070,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.25"/>
@@ -3049,7 +3081,7 @@
     <col min="1" max="1" width="16.21875" customWidth="1"/>
     <col min="2" max="2" width="8.44140625" customWidth="1"/>
     <col min="4" max="4" width="12.21875" customWidth="1"/>
-    <col min="6" max="6" width="25" customWidth="1"/>
+    <col min="6" max="6" width="31.21875" customWidth="1"/>
     <col min="7" max="7" width="21.33203125" customWidth="1"/>
     <col min="9" max="9" width="21.109375" customWidth="1"/>
   </cols>
@@ -3148,14 +3180,80 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="E11" s="32" t="s">
-        <v>52</v>
+      <c r="E11" s="36" t="s">
+        <v>61</v>
       </c>
       <c r="F11" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="G11" s="36" t="s">
+      <c r="G11" s="37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="E12" s="36" t="s">
         <v>61</v>
+      </c>
+      <c r="F12" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="37">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="E13" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" s="37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="E14" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" s="37">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="E15" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="G15" s="39" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="E16" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="G16" s="32">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="17" spans="5:7">
+      <c r="E17" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" s="39" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>